<commit_message>
create ram user from execl
</commit_message>
<xml_diff>
--- a/aliyun_ram/group.xlsx
+++ b/aliyun_ram/group.xlsx
@@ -339,138 +339,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>billing-squad</v>
+        <v>china-infra</v>
       </c>
       <c r="B1" t="str">
-        <v>StagingSwarmAccess,ProductionSwarmAccess,BillingSquadOssPolicy,BillingSquadCdnPolicy,ChinaSpacestationOssPolicy,</v>
+        <v>AdministratorAccess,</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>engagement</v>
+        <v>group-go</v>
       </c>
       <c r="B2" t="str">
-        <v>AliyunMQPubOnlyAccess,AliyunMQSubOnlyAccess,AliyunContainerRegistryReadOnlyAccess,StagingEngagementOSSAccess,ContainerRegistryPullPushAccess,StagingSwarmAccess,</v>
+        <v>AliyunLogReadOnlyAccess,AliyunCloudMonitorReadOnlyAccess,AliyunDysmsReadOnlyAccess,ContainerRegistryPullPushAccess,StagingSwarmAccess,GoSquadCdnPolicy,GoSquadOssPolicy,</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>java</v>
+        <v>ruby</v>
       </c>
       <c r="B3" t="str">
-        <v>AliyunOSSReadOnlyAccess,AliyunLogReadOnlyAccess,AliyunCSReadOnlyAccess,AliyunContainerRegistryFullAccess,AliyunMQReadOnlyAccess,</v>
+        <v>AliyunRDSReadOnlyAccess,AliyunLogReadOnlyAccess,AliyunCSReadOnlyAccess,AliyunContainerRegistryFullAccess,StagingRDSFullAccess,</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>dev-platform</v>
+        <v>java</v>
       </c>
       <c r="B4" t="str">
-        <v>AdministratorAccess,ContainerRegistryPullPushAccess,</v>
+        <v>AliyunOSSReadOnlyAccess,AliyunLogReadOnlyAccess,AliyunCSReadOnlyAccess,AliyunContainerRegistryFullAccess,AliyunMQReadOnlyAccess,java_custom,</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>group-member-to-space</v>
+        <v>billing-squad</v>
       </c>
       <c r="B5" t="str">
-        <v>AliyunLogReadOnlyAccess,AliyunCloudMonitorReadOnlyAccess,StagingSwarmAccess,M2SSquadOssPolicy,M2SSquadCdnPolicy,</v>
+        <v>StagingSwarmAccess,ProductionSwarmAccess,BillingSquadOssPolicy,BillingSquadCdnPolicy,ChinaSpacestationOssPolicy,</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>growth-and-billing-admin</v>
+        <v>engagement</v>
       </c>
       <c r="B6" t="str">
-        <v>AliyunOSSFullAccess,AliyunRDSFullAccess,AliyunKvstoreFullAccess,AliyunCloudMonitorFullAccess,AliyunDysmsFullAccess,AliyunContainerRegistryFullAccess,ListRAMUsers,ProductionSwarmAccess,</v>
+        <v>AliyunMQPubOnlyAccess,AliyunMQSubOnlyAccess,AliyunContainerRegistryReadOnlyAccess,StagingEngagementOSSAccess,ContainerRegistryPullPushAccess,StagingSwarmAccess,</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>recommendation-squad</v>
+        <v>group-member-to-member</v>
       </c>
       <c r="B7" t="str">
-        <v>ContainerRegistryPullPushAccess,</v>
+        <v>AliyunLogReadOnlyAccess,AliyunCloudMonitorReadOnlyAccess,AliyunDysmsReadOnlyAccess,ContainerRegistryPullPushAccess,StagingSwarmAccess,M2MSquadOssPolicy,M2MSquadCdnPolicy,</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>ruby</v>
+        <v>growth-and-billing</v>
       </c>
       <c r="B8" t="str">
-        <v>AliyunRDSReadOnlyAccess,AliyunLogReadOnlyAccess,AliyunCSReadOnlyAccess,AliyunContainerRegistryFullAccess,StagingRDSFullAccess,</v>
+        <v>AliyunContainerRegistryReadOnlyAccess,StagingWWWOSSAccess,StagingRDSFullAccess,ContainerRegistryPullPushAccess,ProductionWWWOSSAccess,StagingSwarmAccess,</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>engagement-admin</v>
+        <v>growth-and-billing-admin</v>
       </c>
       <c r="B9" t="str">
-        <v>StagingECSROAccess,ProductionECSROAccess,StagingSwarmAccess,ProductionSwarmAccess,</v>
+        <v>AliyunOSSFullAccess,AliyunRDSFullAccess,AliyunKvstoreFullAccess,AliyunCloudMonitorFullAccess,AliyunDysmsFullAccess,AliyunContainerRegistryFullAccess,ListRAMUsers,ProductionSwarmAccess,</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>growth-and-billing</v>
+        <v>bastion-operation</v>
       </c>
       <c r="B10" t="str">
-        <v>AliyunContainerRegistryReadOnlyAccess,StagingWWWOSSAccess,StagingRDSFullAccess,ContainerRegistryPullPushAccess,ProductionWWWOSSAccess,StagingSwarmAccess,</v>
+        <v>AliyunYundunBastionHostReadOnlyAccess,AliyunYundunBastionHostOperateOnlyAccess,</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>china-infra</v>
+        <v>china-data-squad</v>
       </c>
       <c r="B11" t="str">
-        <v>AdministratorAccess,</v>
+        <v>AliyunRDSReadOnlyAccess,AliyunDataWorksFullAccess,</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>china-spacestation-developers</v>
+        <v>group-member-to-space</v>
       </c>
       <c r="B12" t="str">
-        <v>ChinaSpacestationOssPolicy,</v>
+        <v>AliyunLogReadOnlyAccess,AliyunCloudMonitorReadOnlyAccess,StagingSwarmAccess,M2SSquadOssPolicy,M2SSquadCdnPolicy,</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>group-go</v>
+        <v>growth-squad</v>
       </c>
       <c r="B13" t="str">
-        <v>AliyunLogReadOnlyAccess,AliyunCloudMonitorReadOnlyAccess,AliyunDysmsReadOnlyAccess,ContainerRegistryPullPushAccess,StagingSwarmAccess,GoSquadCdnPolicy,GoSquadOssPolicy,</v>
+        <v>AliyunLogReadOnlyAccess,AliyunCloudMonitorReadOnlyAccess,AliyunDysmsReadOnlyAccess,ContainerRegistryPullPushAccess,StagingSwarmAccess,GrowthSquadOssPolicy,GrowthSquadCdnPolicy,</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>group-member-to-member</v>
+        <v>recommendation-squad</v>
       </c>
       <c r="B14" t="str">
-        <v>AliyunLogReadOnlyAccess,AliyunCloudMonitorReadOnlyAccess,AliyunDysmsReadOnlyAccess,ContainerRegistryPullPushAccess,StagingSwarmAccess,M2MSquadOssPolicy,M2MSquadCdnPolicy,</v>
+        <v>ContainerRegistryPullPushAccess,</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>growth-squad</v>
+        <v>china-spacestation-developers</v>
       </c>
       <c r="B15" t="str">
-        <v>AliyunLogReadOnlyAccess,AliyunCloudMonitorReadOnlyAccess,AliyunDysmsReadOnlyAccess,ContainerRegistryPullPushAccess,StagingSwarmAccess,GrowthSquadOssPolicy,GrowthSquadCdnPolicy,</v>
+        <v>ChinaSpacestationOssPolicy,</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>bastion-operation</v>
+        <v>dev-platform</v>
       </c>
       <c r="B16" t="str">
-        <v>AliyunYundunBastionHostReadOnlyAccess,AliyunYundunBastionHostOperateOnlyAccess,</v>
+        <v>AdministratorAccess,ContainerRegistryPullPushAccess,</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>china-data-squad</v>
+        <v>engagement-admin</v>
       </c>
       <c r="B17" t="str">
-        <v>AliyunRDSReadOnlyAccess,AliyunDataWorksFullAccess,</v>
+        <v>StagingECSROAccess,ProductionECSROAccess,StagingSwarmAccess,ProductionSwarmAccess,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>